<commit_message>
From this version, I gave a generated system to Marloes Dijkstra.
</commit_message>
<xml_diff>
--- a/WODC/Onderzoeksresultaten.xlsx
+++ b/WODC/Onderzoeksresultaten.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="11112"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="11112" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
     <sheet name="Bronnen" sheetId="2" r:id="rId2"/>
     <sheet name="Beginselen" sheetId="3" r:id="rId3"/>
-    <sheet name="Blad1" sheetId="4" r:id="rId4"/>
+    <sheet name="Definities" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="146">
   <si>
     <t>ICTontwikkeling</t>
   </si>
@@ -28,36 +28,12 @@
     <t>[Beginsel]</t>
   </si>
   <si>
-    <t>voorkomen van eigenrichting</t>
-  </si>
-  <si>
-    <t>respect voor burgerrechten</t>
-  </si>
-  <si>
-    <t>betrouwbare informatie</t>
-  </si>
-  <si>
-    <t>authentieke informatie</t>
-  </si>
-  <si>
-    <t>benodigde informatie</t>
-  </si>
-  <si>
-    <t>duurzame informatie</t>
-  </si>
-  <si>
-    <t>welke zeggenschap heeft de burger over informatie?</t>
-  </si>
-  <si>
     <t>menselijke maat</t>
   </si>
   <si>
     <t>balans tussen mens en machine</t>
   </si>
   <si>
-    <t>bereikbare informatie</t>
-  </si>
-  <si>
     <t>beheer bij de bron</t>
   </si>
   <si>
@@ -79,9 +55,6 @@
     <t>equality of arms</t>
   </si>
   <si>
-    <t xml:space="preserve">berechting op tegenspraak </t>
-  </si>
-  <si>
     <t>respect voor discretionaire bevoegdheden</t>
   </si>
   <si>
@@ -94,27 +67,15 @@
     <t>doelbinding</t>
   </si>
   <si>
-    <t>adequate bijstand</t>
-  </si>
-  <si>
     <t>tijdigheid</t>
   </si>
   <si>
-    <t>externe openbaarheid</t>
-  </si>
-  <si>
     <t>j</t>
   </si>
   <si>
-    <t xml:space="preserve">interne openbaarheid </t>
-  </si>
-  <si>
     <t>uniformering vanuit regelgeving</t>
   </si>
   <si>
-    <t>consistente informatie</t>
-  </si>
-  <si>
     <t>De informatie is vrij van redundantie.</t>
   </si>
   <si>
@@ -187,9 +148,6 @@
     <t>Regels, die zorgen dat vanuit een gegeven verzameling feiten</t>
   </si>
   <si>
-    <t>objectieve informatie</t>
-  </si>
-  <si>
     <t xml:space="preserve">Van objectieve informatie mag redelijkerwijs worden aangenomen dat </t>
   </si>
   <si>
@@ -211,24 +169,15 @@
     <t>een uitspraak, die in een zekere context als waar geldt.</t>
   </si>
   <si>
-    <t>Cloud</t>
-  </si>
-  <si>
     <t>alomtegenwoordige informatie</t>
   </si>
   <si>
     <t>zaak</t>
   </si>
   <si>
-    <t>relevante informatie</t>
-  </si>
-  <si>
     <t>De informatie beïnvloedt het bereiken van een zeker doel</t>
   </si>
   <si>
-    <t>internet of everything</t>
-  </si>
-  <si>
     <t>unified communication</t>
   </si>
   <si>
@@ -335,13 +284,184 @@
   </si>
   <si>
     <t>Onder "semantische technologie" wordt verstaan alle technologie, die in staat is om een vooraf bedoelde betekenis te geven aan menselijke uitingen.</t>
+  </si>
+  <si>
+    <t>[PersonReg]</t>
+  </si>
+  <si>
+    <t>personFirstName</t>
+  </si>
+  <si>
+    <t>personLastName</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Stef Joosten</t>
+  </si>
+  <si>
+    <t>Stef</t>
+  </si>
+  <si>
+    <t>Joosten</t>
+  </si>
+  <si>
+    <t>Marloes Dijkstra</t>
+  </si>
+  <si>
+    <t>Marloes</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
+    <t>Mark Visser</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Visser</t>
+  </si>
+  <si>
+    <t>Evert Stamhuis</t>
+  </si>
+  <si>
+    <t>Evert</t>
+  </si>
+  <si>
+    <t>Stamhuis</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>stef.joosten@ou.nl</t>
+  </si>
+  <si>
+    <t>0651348895</t>
+  </si>
+  <si>
+    <t>Frits Bussemaker</t>
+  </si>
+  <si>
+    <t>CIONET Nederland</t>
+  </si>
+  <si>
+    <t>+316 11045050</t>
+  </si>
+  <si>
+    <t>frits@bussemaker.net</t>
+  </si>
+  <si>
+    <t>[OrganizationReg]</t>
+  </si>
+  <si>
+    <t>orgAbbrName</t>
+  </si>
+  <si>
+    <t>orgFullName</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>OrgAbbrName</t>
+  </si>
+  <si>
+    <t>OrgFullName</t>
+  </si>
+  <si>
+    <t>OUNL</t>
+  </si>
+  <si>
+    <t>Open Universiteit Nederland</t>
+  </si>
+  <si>
+    <t>CIONET</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>Ordina</t>
+  </si>
+  <si>
+    <t>Organisatie</t>
+  </si>
+  <si>
+    <t>Telefoon</t>
+  </si>
+  <si>
+    <t>bellen</t>
+  </si>
+  <si>
+    <t>Frits</t>
+  </si>
+  <si>
+    <t>Bussemaker</t>
+  </si>
+  <si>
+    <t>internet of things</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>Legaliteit</t>
+  </si>
+  <si>
+    <t>Externe openbaarheid</t>
+  </si>
+  <si>
+    <t>Onafhankelijkheid</t>
+  </si>
+  <si>
+    <t>Betrouwbaarheid/behoorlijkheid</t>
+  </si>
+  <si>
+    <t>[Begrip]</t>
+  </si>
+  <si>
+    <t>betrouwbaar</t>
+  </si>
+  <si>
+    <t>authentiek</t>
+  </si>
+  <si>
+    <t>consistent</t>
+  </si>
+  <si>
+    <t>benodigd</t>
+  </si>
+  <si>
+    <t>objectief</t>
+  </si>
+  <si>
+    <t>duurzam</t>
+  </si>
+  <si>
+    <t>bereikbaar</t>
+  </si>
+  <si>
+    <t>relevant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,16 +476,41 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,23 +518,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Berekening" xfId="3" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutraal" xfId="2" builtinId="28"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -684,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -699,25 +882,25 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -725,22 +908,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.8">
@@ -748,16 +931,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2">
@@ -765,19 +948,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8">
@@ -785,13 +968,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8">
@@ -799,13 +982,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8">
@@ -813,19 +996,19 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2">
@@ -833,10 +1016,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2">
@@ -844,16 +1027,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6">
@@ -861,13 +1044,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.2">
@@ -875,16 +1058,16 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -895,22 +1078,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -924,16 +1294,16 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -941,16 +1311,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -958,10 +1328,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -969,10 +1339,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -980,10 +1350,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -991,10 +1361,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1002,10 +1372,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1013,343 +1383,178 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29">
-        <v>27</v>
-      </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1562,7 @@
     <sortCondition ref="C3:C27"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E28" r:id="rId1" tooltip="Europees Verdrag voor de Rechten van de Mens" display="https://nl.wikipedia.org/wiki/Europees_Verdrag_voor_de_Rechten_van_de_Mens"/>
+    <hyperlink ref="E25" r:id="rId1" tooltip="Europees Verdrag voor de Rechten van de Mens" display="https://nl.wikipedia.org/wiki/Europees_Verdrag_voor_de_Rechten_van_de_Mens"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1366,12 +1571,186 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="93.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further work on WODC
</commit_message>
<xml_diff>
--- a/WODC/Onderzoeksresultaten.xlsx
+++ b/WODC/Onderzoeksresultaten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="11112" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="20730" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
-    <sheet name="Bronnen" sheetId="2" r:id="rId2"/>
+    <sheet name="Deelnemers" sheetId="2" r:id="rId2"/>
     <sheet name="Beginselen" sheetId="3" r:id="rId3"/>
     <sheet name="Definities" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -460,8 +460,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,11 +577,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -655,6 +660,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -689,6 +695,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -864,23 +871,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="47.109375" customWidth="1"/>
-    <col min="7" max="7" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -903,7 +910,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -926,7 +933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="100.8">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -943,7 +950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -963,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -977,7 +984,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -991,7 +998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1011,7 +1018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1022,7 +1029,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="57.6">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1077,20 +1084,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>89</v>
       </c>
@@ -1110,7 +1117,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>95</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -1164,7 +1171,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>101</v>
       </c>
@@ -1178,7 +1185,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>104</v>
       </c>
@@ -1192,7 +1199,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>115</v>
       </c>
@@ -1223,7 +1230,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>118</v>
       </c>
@@ -1234,7 +1241,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>121</v>
       </c>
@@ -1245,7 +1252,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -1276,20 +1283,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1306,7 +1313,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1323,7 +1330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1356,7 +1363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1378,7 +1385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1389,7 +1396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -1431,7 +1438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>22</v>
       </c>
@@ -1445,7 +1452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>23</v>
       </c>
@@ -1459,7 +1466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24</v>
       </c>
@@ -1473,7 +1480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>28</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>29</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>51</v>
       </c>
@@ -1570,21 +1577,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="93.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="93.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -1601,7 +1608,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1618,7 +1625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1635,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -1649,7 +1656,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
@@ -1666,7 +1673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -1680,7 +1687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1708,7 +1715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>

</xml_diff>